<commit_message>
error bars community comp figures
</commit_message>
<xml_diff>
--- a/data/2024-03-06_data_for_stacked_plots.xlsx
+++ b/data/2024-03-06_data_for_stacked_plots.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\OneDrive\Desktop\MS Thesis\MS_Thesis_2023-2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C078047C-4838-4A3C-9BF4-6BC27A1B95A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB320C3-D9F0-4498-99CF-0E378DB5C3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" firstSheet="3" activeTab="3" xr2:uid="{35F6197A-F48F-4BA3-A374-5C0663C6D00B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="3" activeTab="4" xr2:uid="{35F6197A-F48F-4BA3-A374-5C0663C6D00B}"/>
   </bookViews>
   <sheets>
     <sheet name="Biomass" sheetId="1" r:id="rId1"/>
     <sheet name="Biomass_dh" sheetId="4" r:id="rId2"/>
     <sheet name="Percent_Change" sheetId="2" r:id="rId3"/>
     <sheet name="Percent_Change_dh" sheetId="3" r:id="rId4"/>
+    <sheet name="Percent_Change_dh_sd" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="24">
   <si>
     <t>Treatment</t>
   </si>
@@ -99,6 +100,18 @@
   </si>
   <si>
     <t>dh</t>
+  </si>
+  <si>
+    <t>B1_sd</t>
+  </si>
+  <si>
+    <t>B2_sd</t>
+  </si>
+  <si>
+    <t>B3_sd</t>
+  </si>
+  <si>
+    <t>B4_sd</t>
   </si>
 </sst>
 </file>
@@ -2739,20 +2752,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47899AAC-7D4F-4CC6-80E7-C741569B9C77}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2763,16 +2782,28 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2782,17 +2813,29 @@
       <c r="C2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E2">
         <v>24.991034466290163</v>
       </c>
-      <c r="E2">
+      <c r="F2">
+        <v>38.28275</v>
+      </c>
+      <c r="G2">
         <v>8.020726673135016</v>
       </c>
-      <c r="F2">
+      <c r="H2">
+        <v>10.236269999999999</v>
+      </c>
+      <c r="I2">
         <v>125.59053472411998</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>52.403790000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2802,17 +2845,17 @@
       <c r="C3">
         <v>405.27408991682103</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>558.04633250803704</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>366.38746698215277</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>44.060717143881888</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2823,16 +2866,19 @@
         <v>398.72953549933618</v>
       </c>
       <c r="D4">
+        <v>105.860719</v>
+      </c>
+      <c r="E4">
         <v>1005.7434122593631</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>165.53579316898487</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>77.024904958955347</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2842,17 +2888,17 @@
       <c r="C5">
         <v>-84.565128172239071</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-67.187680550985561</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>18.243521817957895</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>2290.9299128885586</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2862,19 +2908,19 @@
       <c r="C6">
         <v>550.28761006373304</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>673.50362818064912</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>616.97860943268665</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>647.34079780027582</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -2882,99 +2928,114 @@
       <c r="C7" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D7">
-        <v>-14.507008921438663</v>
+      <c r="D7" t="e">
+        <v>#DIV/0!</v>
       </c>
       <c r="E7">
-        <v>-3.017728836240591</v>
+        <v>-100</v>
       </c>
       <c r="F7">
-        <v>99.782005975684626</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>36.314950227629943</v>
+      </c>
+      <c r="H7">
+        <v>10.66999</v>
+      </c>
+      <c r="I7">
+        <v>124.34455988228237</v>
+      </c>
+      <c r="J7">
+        <v>31.01952</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>8.3009730475515724</v>
-      </c>
-      <c r="D8">
-        <v>15.654922129610686</v>
+        <v>460.15717241083303</v>
       </c>
       <c r="E8">
-        <v>8.952739591023402</v>
-      </c>
-      <c r="F8">
-        <v>48.415557853258044</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1111.18706007129</v>
+      </c>
+      <c r="G8">
+        <v>335.84192630517202</v>
+      </c>
+      <c r="I8">
+        <v>22.378177317166756</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9">
-        <v>54.611500858713875</v>
+        <v>491.67748135388655</v>
       </c>
       <c r="D9">
-        <v>52.053874275357899</v>
+        <v>53.632336000000002</v>
       </c>
       <c r="E9">
-        <v>2.1118988071661127</v>
-      </c>
-      <c r="F9">
-        <v>13.423894088760557</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1238.5691494209455</v>
+      </c>
+      <c r="G9">
+        <v>198.83426514184617</v>
+      </c>
+      <c r="I9">
+        <v>78.287744328065358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10">
-        <v>-99.477442334586698</v>
-      </c>
-      <c r="D10">
-        <v>2.8370873337977853</v>
+        <v>-6.4523183975711715</v>
       </c>
       <c r="E10">
-        <v>8.1360869269716325</v>
-      </c>
-      <c r="F10">
-        <v>204.37062349714557</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>437.36520007762829</v>
+      </c>
+      <c r="G10">
+        <v>122.14509730079324</v>
+      </c>
+      <c r="I10">
+        <v>2279.8838190622564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C11">
-        <v>53.987685411963128</v>
-      </c>
-      <c r="D11">
-        <v>56.709150744292643</v>
+        <v>808.08221906215044</v>
       </c>
       <c r="E11">
-        <v>32.615716189125763</v>
-      </c>
-      <c r="F11">
-        <v>64.602346051952878</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1509.8576569207023</v>
+      </c>
+      <c r="G11">
+        <v>641.84863983170192</v>
+      </c>
+      <c r="I11">
+        <v>487.90450677072693</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -2982,99 +3043,114 @@
       <c r="C12" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D12">
-        <v>2.4634902796250331</v>
+      <c r="D12" t="e">
+        <v>#DIV/0!</v>
       </c>
       <c r="E12">
-        <v>11.413203679606063</v>
+        <v>-100</v>
       </c>
       <c r="F12">
-        <v>109.39822636182961</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>23.829474671855277</v>
+      </c>
+      <c r="H12">
+        <v>54.478079999999999</v>
+      </c>
+      <c r="I12">
+        <v>141.82707723156733</v>
+      </c>
+      <c r="J12">
+        <v>35.880470000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C13">
-        <v>3.5182518152847635</v>
-      </c>
-      <c r="D13">
-        <v>16.152860713874457</v>
+        <v>402.5305938225431</v>
       </c>
       <c r="E13">
-        <v>-7.6644056939665344</v>
-      </c>
-      <c r="F13">
-        <v>14.848040588937574</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1027.2938044544999</v>
+      </c>
+      <c r="G13">
+        <v>302.0544966403188</v>
+      </c>
+      <c r="I13">
+        <v>28.776322413542562</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C14">
-        <v>42.850414978902947</v>
+        <v>406.45332701113466</v>
       </c>
       <c r="D14">
-        <v>13.243557279176073</v>
+        <v>153.95881299999999</v>
       </c>
       <c r="E14">
-        <v>-7.559072165529887E-2</v>
-      </c>
-      <c r="F14">
-        <v>7.0493740645689131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1205.6139627049101</v>
+      </c>
+      <c r="G14">
+        <v>193.50788822116579</v>
+      </c>
+      <c r="I14">
+        <v>75.825243550960806</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15">
-        <v>-57.863493445218793</v>
-      </c>
-      <c r="D15">
-        <v>-81.968508522282221</v>
+        <v>-89.970254080785338</v>
       </c>
       <c r="E15">
-        <v>98.028707440163629</v>
-      </c>
-      <c r="F15">
-        <v>-0.50103107696689331</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>359.7648399876212</v>
+      </c>
+      <c r="G15">
+        <v>410.91741950787957</v>
+      </c>
+      <c r="I15">
+        <v>1717.9651953326575</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C16">
-        <v>27.985412742771523</v>
-      </c>
-      <c r="D16">
-        <v>45.95600195930944</v>
+        <v>585.95227980455661</v>
       </c>
       <c r="E16">
-        <v>36.767456175614889</v>
-      </c>
-      <c r="F16">
-        <v>36.767456175614889</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1446.8361107439159</v>
+      </c>
+      <c r="G16">
+        <v>531.8419756963491</v>
+      </c>
+      <c r="I16">
+        <v>484.83071456682683</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -3082,99 +3158,114 @@
       <c r="C17" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D17">
-        <v>-100</v>
+      <c r="D17" t="e">
+        <v>#DIV/0!</v>
       </c>
       <c r="E17">
-        <v>23.829474671855277</v>
+        <v>2.4634902796250331</v>
       </c>
       <c r="F17">
-        <v>141.82707723156733</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>33.042430000000003</v>
+      </c>
+      <c r="G17">
+        <v>11.413203679606063</v>
+      </c>
+      <c r="H17">
+        <v>10.36322</v>
+      </c>
+      <c r="I17">
+        <v>109.39822636182961</v>
+      </c>
+      <c r="J17">
+        <v>92.957120000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C18">
-        <v>402.5305938225431</v>
-      </c>
-      <c r="D18">
-        <v>1027.2938044544999</v>
+        <v>3.5182518152847635</v>
       </c>
       <c r="E18">
-        <v>302.0544966403188</v>
-      </c>
-      <c r="F18">
-        <v>28.776322413542562</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16.152860713874457</v>
+      </c>
+      <c r="G18">
+        <v>-7.6644056939665344</v>
+      </c>
+      <c r="I18">
+        <v>14.848040588937574</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C19">
-        <v>406.45332701113466</v>
+        <v>42.850414978902947</v>
       </c>
       <c r="D19">
-        <v>1205.6139627049101</v>
+        <v>29.531212</v>
       </c>
       <c r="E19">
-        <v>193.50788822116579</v>
-      </c>
-      <c r="F19">
-        <v>75.825243550960806</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13.243557279176073</v>
+      </c>
+      <c r="G19">
+        <v>-7.559072165529887E-2</v>
+      </c>
+      <c r="I19">
+        <v>7.0493740645689131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20">
-        <v>-89.970254080785338</v>
-      </c>
-      <c r="D20">
-        <v>359.7648399876212</v>
+        <v>-57.863493445218793</v>
       </c>
       <c r="E20">
-        <v>410.91741950787957</v>
-      </c>
-      <c r="F20">
-        <v>1717.9651953326575</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-81.968508522282221</v>
+      </c>
+      <c r="G20">
+        <v>98.028707440163629</v>
+      </c>
+      <c r="I20">
+        <v>-0.50103107696689331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C21">
-        <v>585.95227980455661</v>
-      </c>
-      <c r="D21">
-        <v>1446.8361107439159</v>
+        <v>27.985412742771523</v>
       </c>
       <c r="E21">
-        <v>531.8419756963491</v>
-      </c>
-      <c r="F21">
-        <v>484.83071456682683</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>45.95600195930944</v>
+      </c>
+      <c r="G21">
+        <v>36.767456175614889</v>
+      </c>
+      <c r="I21">
+        <v>36.767456175614889</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>3</v>
@@ -3182,94 +3273,967 @@
       <c r="C22" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="D22">
-        <v>-100</v>
+      <c r="D22" t="e">
+        <v>#DIV/0!</v>
       </c>
       <c r="E22">
-        <v>36.314950227629943</v>
+        <v>-14.507008921438663</v>
       </c>
       <c r="F22">
-        <v>124.34455988228237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>38.59787</v>
+      </c>
+      <c r="G22">
+        <v>-3.017728836240591</v>
+      </c>
+      <c r="H22">
+        <v>15.655620000000001</v>
+      </c>
+      <c r="I22">
+        <v>99.782005975684626</v>
+      </c>
+      <c r="J22">
+        <v>117.79443999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C23">
-        <v>460.15717241083303</v>
-      </c>
-      <c r="D23">
-        <v>1111.18706007129</v>
+        <v>8.3009730475515724</v>
       </c>
       <c r="E23">
-        <v>335.84192630517202</v>
-      </c>
-      <c r="F23">
-        <v>22.378177317166756</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15.654922129610686</v>
+      </c>
+      <c r="G23">
+        <v>8.952739591023402</v>
+      </c>
+      <c r="I23">
+        <v>48.415557853258044</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C24">
-        <v>491.67748135388655</v>
+        <v>54.611500858713875</v>
       </c>
       <c r="D24">
-        <v>1238.5691494209455</v>
+        <v>42.611066999999998</v>
       </c>
       <c r="E24">
-        <v>198.83426514184617</v>
-      </c>
-      <c r="F24">
-        <v>78.287744328065358</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>52.053874275357899</v>
+      </c>
+      <c r="G24">
+        <v>2.1118988071661127</v>
+      </c>
+      <c r="I24">
+        <v>13.423894088760557</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25">
-        <v>-6.4523183975711715</v>
-      </c>
-      <c r="D25">
-        <v>437.36520007762829</v>
+        <v>-99.477442334586698</v>
       </c>
       <c r="E25">
-        <v>122.14509730079324</v>
-      </c>
-      <c r="F25">
-        <v>2279.8838190622564</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2.8370873337977853</v>
+      </c>
+      <c r="G25">
+        <v>8.1360869269716325</v>
+      </c>
+      <c r="I25">
+        <v>204.37062349714557</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C26">
+        <v>53.987685411963128</v>
+      </c>
+      <c r="E26">
+        <v>56.709150744292643</v>
+      </c>
+      <c r="G26">
+        <v>32.615716189125763</v>
+      </c>
+      <c r="I26">
+        <v>64.602346051952878</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691C3427-274E-4B52-B768-D4251A401BD4}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E2">
+        <v>24.991034466290163</v>
+      </c>
+      <c r="F2">
+        <v>38.28275</v>
+      </c>
+      <c r="G2">
+        <v>8.020726673135016</v>
+      </c>
+      <c r="H2">
+        <v>10.236269999999999</v>
+      </c>
+      <c r="I2">
+        <v>125.59053472411998</v>
+      </c>
+      <c r="J2">
+        <v>52.403790000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>405.27408991682103</v>
+      </c>
+      <c r="D3">
+        <v>152.50990200000001</v>
+      </c>
+      <c r="E3">
+        <v>558.04633250803704</v>
+      </c>
+      <c r="F3">
+        <v>103.58918300000001</v>
+      </c>
+      <c r="G3">
+        <v>366.38746698215277</v>
+      </c>
+      <c r="H3">
+        <v>68.896709000000001</v>
+      </c>
+      <c r="I3">
+        <v>44.060717143881888</v>
+      </c>
+      <c r="J3">
+        <v>12.620718999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>398.72953549933618</v>
+      </c>
+      <c r="D4">
+        <v>105.860719</v>
+      </c>
+      <c r="E4">
+        <v>1005.7434122593631</v>
+      </c>
+      <c r="F4">
+        <v>47.466428000000001</v>
+      </c>
+      <c r="G4">
+        <v>165.53579316898487</v>
+      </c>
+      <c r="H4">
+        <v>17.851455999999999</v>
+      </c>
+      <c r="I4">
+        <v>77.024904958955347</v>
+      </c>
+      <c r="J4">
+        <v>9.278613</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>-84.565128172239071</v>
+      </c>
+      <c r="D5">
+        <v>16.100065300000001</v>
+      </c>
+      <c r="E5">
+        <v>-67.187680550985561</v>
+      </c>
+      <c r="F5">
+        <v>38.979690599999998</v>
+      </c>
+      <c r="G5">
+        <v>18.243521817957895</v>
+      </c>
+      <c r="H5">
+        <v>33.002187999999997</v>
+      </c>
+      <c r="I5">
+        <v>2290.9299128885586</v>
+      </c>
+      <c r="J5">
+        <v>721.08204350000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>550.28761006373304</v>
+      </c>
+      <c r="D6">
+        <v>147.44527299999999</v>
+      </c>
+      <c r="E6">
+        <v>673.50362818064912</v>
+      </c>
+      <c r="F6">
+        <v>32.127330999999998</v>
+      </c>
+      <c r="G6">
+        <v>616.97860943268665</v>
+      </c>
+      <c r="H6">
+        <v>71.681352000000004</v>
+      </c>
+      <c r="I6">
+        <v>647.34079780027582</v>
+      </c>
+      <c r="J6">
+        <v>56.012467000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D7" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7">
+        <v>-100</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>36.314950227629943</v>
+      </c>
+      <c r="H7">
+        <v>10.66999</v>
+      </c>
+      <c r="I7">
+        <v>124.34455988228237</v>
+      </c>
+      <c r="J7">
+        <v>31.01952</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>460.15717241083303</v>
+      </c>
+      <c r="D8">
+        <v>186.62494100000001</v>
+      </c>
+      <c r="E8">
+        <v>1111.18706007129</v>
+      </c>
+      <c r="F8">
+        <v>87.932171999999994</v>
+      </c>
+      <c r="G8">
+        <v>335.84192630517202</v>
+      </c>
+      <c r="H8">
+        <v>69.657369000000003</v>
+      </c>
+      <c r="I8">
+        <v>22.378177317166756</v>
+      </c>
+      <c r="J8">
+        <v>22.109687000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>491.67748135388655</v>
+      </c>
+      <c r="D9">
+        <v>53.632336000000002</v>
+      </c>
+      <c r="E9">
+        <v>1238.5691494209455</v>
+      </c>
+      <c r="F9">
+        <v>125.90683199999999</v>
+      </c>
+      <c r="G9">
+        <v>198.83426514184617</v>
+      </c>
+      <c r="H9">
+        <v>63.567964000000003</v>
+      </c>
+      <c r="I9">
+        <v>78.287744328065358</v>
+      </c>
+      <c r="J9">
+        <v>9.8094260000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>-6.4523183975711715</v>
+      </c>
+      <c r="D10">
+        <v>163.08657880000001</v>
+      </c>
+      <c r="E10">
+        <v>437.36520007762829</v>
+      </c>
+      <c r="F10">
+        <v>117.4458451</v>
+      </c>
+      <c r="G10">
+        <v>122.14509730079324</v>
+      </c>
+      <c r="H10">
+        <v>136.91773660000001</v>
+      </c>
+      <c r="I10">
+        <v>2279.8838190622564</v>
+      </c>
+      <c r="J10">
+        <v>1178.8060627</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
         <v>808.08221906215044</v>
       </c>
+      <c r="D11">
+        <v>112.88736900000001</v>
+      </c>
+      <c r="E11">
+        <v>1509.8576569207023</v>
+      </c>
+      <c r="F11">
+        <v>46.295085</v>
+      </c>
+      <c r="G11">
+        <v>641.84863983170192</v>
+      </c>
+      <c r="H11">
+        <v>57.873102000000003</v>
+      </c>
+      <c r="I11">
+        <v>487.90450677072693</v>
+      </c>
+      <c r="J11">
+        <v>68.037246999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D12" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12">
+        <v>-100</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>23.829474671855277</v>
+      </c>
+      <c r="H12">
+        <v>54.478079999999999</v>
+      </c>
+      <c r="I12">
+        <v>141.82707723156733</v>
+      </c>
+      <c r="J12">
+        <v>35.880470000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>402.5305938225431</v>
+      </c>
+      <c r="D13">
+        <v>181.44875999999999</v>
+      </c>
+      <c r="E13">
+        <v>1027.2938044544999</v>
+      </c>
+      <c r="F13">
+        <v>76.880734000000004</v>
+      </c>
+      <c r="G13">
+        <v>302.0544966403188</v>
+      </c>
+      <c r="H13">
+        <v>107.931562</v>
+      </c>
+      <c r="I13">
+        <v>28.776322413542562</v>
+      </c>
+      <c r="J13">
+        <v>15.406814000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>406.45332701113466</v>
+      </c>
+      <c r="D14">
+        <v>153.95881299999999</v>
+      </c>
+      <c r="E14">
+        <v>1205.6139627049101</v>
+      </c>
+      <c r="F14">
+        <v>88.799442999999997</v>
+      </c>
+      <c r="G14">
+        <v>193.50788822116579</v>
+      </c>
+      <c r="H14">
+        <v>43.073157000000002</v>
+      </c>
+      <c r="I14">
+        <v>75.825243550960806</v>
+      </c>
+      <c r="J14">
+        <v>8.2991910000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>-89.970254080785338</v>
+      </c>
+      <c r="D15">
+        <v>14.836558500000001</v>
+      </c>
+      <c r="E15">
+        <v>359.7648399876212</v>
+      </c>
+      <c r="F15">
+        <v>244.87838020000001</v>
+      </c>
+      <c r="G15">
+        <v>410.91741950787957</v>
+      </c>
+      <c r="H15">
+        <v>279.06220739999998</v>
+      </c>
+      <c r="I15">
+        <v>1717.9651953326575</v>
+      </c>
+      <c r="J15">
+        <v>1315.7393578000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>585.95227980455661</v>
+      </c>
+      <c r="D16">
+        <v>180.92465200000001</v>
+      </c>
+      <c r="E16">
+        <v>1446.8361107439159</v>
+      </c>
+      <c r="F16">
+        <v>227.06039200000001</v>
+      </c>
+      <c r="G16">
+        <v>531.8419756963491</v>
+      </c>
+      <c r="H16">
+        <v>154.72507400000001</v>
+      </c>
+      <c r="I16">
+        <v>484.83071456682683</v>
+      </c>
+      <c r="J16">
+        <v>81.524231999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17">
+        <v>2.4634902796250331</v>
+      </c>
+      <c r="F17">
+        <v>33.042430000000003</v>
+      </c>
+      <c r="G17">
+        <v>11.413203679606063</v>
+      </c>
+      <c r="H17">
+        <v>10.36322</v>
+      </c>
+      <c r="I17">
+        <v>109.39822636182961</v>
+      </c>
+      <c r="J17">
+        <v>92.957120000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>3.5182518152847635</v>
+      </c>
+      <c r="D18">
+        <v>7.2682370000000001</v>
+      </c>
+      <c r="E18">
+        <v>16.152860713874457</v>
+      </c>
+      <c r="F18">
+        <v>9.9020109999999999</v>
+      </c>
+      <c r="G18">
+        <v>-7.6644056939665344</v>
+      </c>
+      <c r="H18">
+        <v>7.6755890000000004</v>
+      </c>
+      <c r="I18">
+        <v>14.848040588937574</v>
+      </c>
+      <c r="J18">
+        <v>16.286487000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>42.850414978902947</v>
+      </c>
+      <c r="D19">
+        <v>29.531212</v>
+      </c>
+      <c r="E19">
+        <v>13.243557279176073</v>
+      </c>
+      <c r="F19">
+        <v>53.010331999999998</v>
+      </c>
+      <c r="G19">
+        <v>-7.559072165529887E-2</v>
+      </c>
+      <c r="H19">
+        <v>1.5471950000000001</v>
+      </c>
+      <c r="I19">
+        <v>7.0493740645689131</v>
+      </c>
+      <c r="J19">
+        <v>4.3621020000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>-57.863493445218793</v>
+      </c>
+      <c r="D20">
+        <v>93.915365300000005</v>
+      </c>
+      <c r="E20">
+        <v>-81.968508522282221</v>
+      </c>
+      <c r="F20">
+        <v>36.450913900000003</v>
+      </c>
+      <c r="G20">
+        <v>98.028707440163629</v>
+      </c>
+      <c r="H20">
+        <v>271.21882529999999</v>
+      </c>
+      <c r="I20">
+        <v>-0.50103107696689331</v>
+      </c>
+      <c r="J20">
+        <v>219.87933469999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>27.985412742771523</v>
+      </c>
+      <c r="D21">
+        <v>4.922498</v>
+      </c>
+      <c r="E21">
+        <v>45.95600195930944</v>
+      </c>
+      <c r="F21">
+        <v>14.102129</v>
+      </c>
+      <c r="G21">
+        <v>36.767456175614889</v>
+      </c>
+      <c r="H21">
+        <v>2.7466759999999999</v>
+      </c>
+      <c r="I21">
+        <v>36.767456175614889</v>
+      </c>
+      <c r="J21">
+        <v>17.143992000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D22" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E22">
+        <v>-14.507008921438663</v>
+      </c>
+      <c r="F22">
+        <v>38.59787</v>
+      </c>
+      <c r="G22">
+        <v>-3.017728836240591</v>
+      </c>
+      <c r="H22">
+        <v>15.655620000000001</v>
+      </c>
+      <c r="I22">
+        <v>99.782005975684626</v>
+      </c>
+      <c r="J22">
+        <v>117.79443999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>8.3009730475515724</v>
+      </c>
+      <c r="D23">
+        <v>18.819911999999999</v>
+      </c>
+      <c r="E23">
+        <v>15.654922129610686</v>
+      </c>
+      <c r="F23">
+        <v>14.012916000000001</v>
+      </c>
+      <c r="G23">
+        <v>8.952739591023402</v>
+      </c>
+      <c r="H23">
+        <v>13.043493</v>
+      </c>
+      <c r="I23">
+        <v>48.415557853258044</v>
+      </c>
+      <c r="J23">
+        <v>44.271532999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>54.611500858713875</v>
+      </c>
+      <c r="D24">
+        <v>42.611066999999998</v>
+      </c>
+      <c r="E24">
+        <v>52.053874275357899</v>
+      </c>
+      <c r="F24">
+        <v>38.524794999999997</v>
+      </c>
+      <c r="G24">
+        <v>2.1118988071661127</v>
+      </c>
+      <c r="H24">
+        <v>4.5694090000000003</v>
+      </c>
+      <c r="I24">
+        <v>13.423894088760557</v>
+      </c>
+      <c r="J24">
+        <v>9.1880089999999992</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>-99.477442334586698</v>
+      </c>
+      <c r="D25">
+        <v>0.92347650000000003</v>
+      </c>
+      <c r="E25">
+        <v>2.8370873337977853</v>
+      </c>
+      <c r="F25">
+        <v>227.71391370000001</v>
+      </c>
+      <c r="G25">
+        <v>8.1360869269716325</v>
+      </c>
+      <c r="H25">
+        <v>224.399957</v>
+      </c>
+      <c r="I25">
+        <v>204.37062349714557</v>
+      </c>
+      <c r="J25">
+        <v>298.27074379999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>53.987685411963128</v>
+      </c>
       <c r="D26">
-        <v>1509.8576569207023</v>
+        <v>33.341661000000002</v>
       </c>
       <c r="E26">
-        <v>641.84863983170192</v>
+        <v>56.709150744292643</v>
       </c>
       <c r="F26">
-        <v>487.90450677072693</v>
+        <v>33.066291</v>
+      </c>
+      <c r="G26">
+        <v>32.615716189125763</v>
+      </c>
+      <c r="H26">
+        <v>23.766133</v>
+      </c>
+      <c r="I26">
+        <v>64.602346051952878</v>
+      </c>
+      <c r="J26">
+        <v>47.074567000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>